<commit_message>
Ajustes de escaleta solicitados por Oliver
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/MA_06_04_CO Escaleta.xlsx
+++ b/fuentes/contenidos/grado06/guion04/MA_06_04_CO Escaleta.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="24760" windowHeight="14220" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="365">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1105,6 +1105,18 @@
   </si>
   <si>
     <t>Ejercicios de afianzamiento del mcd y el mcm</t>
+  </si>
+  <si>
+    <t>1º ESO</t>
+  </si>
+  <si>
+    <t>Las operaciones con números naturales</t>
+  </si>
+  <si>
+    <t>MT_07_02</t>
+  </si>
+  <si>
+    <t>Enunciados en los cuales se plantean actividades de problemas sencillos de los conceptos de míltuplis, divisores, mcm y mcd</t>
   </si>
 </sst>
 </file>
@@ -1641,22 +1653,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1693,18 +1717,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6365,8 +6377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G14" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="G12" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6399,104 +6411,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="43" customFormat="1" ht="15">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="94" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="E1" s="86" t="s">
         <v>279</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="84" t="s">
         <v>280</v>
       </c>
       <c r="G1" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="I1" s="82" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="74" t="s">
+      <c r="J1" s="76" t="s">
         <v>202</v>
       </c>
-      <c r="K1" s="86" t="s">
+      <c r="K1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="84" t="s">
+      <c r="M1" s="88" t="s">
         <v>277</v>
       </c>
-      <c r="N1" s="74" t="s">
+      <c r="N1" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="88" t="s">
+      <c r="O1" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="78" t="s">
+      <c r="P1" s="93"/>
+      <c r="Q1" s="74" t="s">
         <v>203</v>
       </c>
-      <c r="R1" s="78" t="s">
+      <c r="R1" s="74" t="s">
         <v>204</v>
       </c>
-      <c r="S1" s="92" t="s">
+      <c r="S1" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="T1" s="94" t="s">
+      <c r="T1" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="U1" s="92" t="s">
+      <c r="U1" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="V1" s="94" t="s">
+      <c r="V1" s="80" t="s">
         <v>126</v>
       </c>
-      <c r="W1" s="92" t="s">
+      <c r="W1" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="Y1" s="74" t="s">
+      <c r="Y1" s="76" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="43" customFormat="1" ht="15">
-      <c r="A2" s="83"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="91"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="95"/>
       <c r="D2" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="81"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="32"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="87"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="75"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="91"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="77"/>
       <c r="O2" s="30" t="s">
         <v>128</v>
       </c>
       <c r="P2" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="93"/>
-      <c r="Y2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="79"/>
+      <c r="Y2" s="77"/>
     </row>
     <row r="3" spans="1:25" s="43" customFormat="1" ht="79" customHeight="1">
       <c r="A3" s="35" t="s">
@@ -7217,11 +7229,21 @@
       <c r="R14" s="50" t="s">
         <v>354</v>
       </c>
-      <c r="S14" s="56"/>
-      <c r="T14" s="56"/>
-      <c r="U14" s="56"/>
-      <c r="V14" s="57"/>
-      <c r="W14" s="56"/>
+      <c r="S14" t="s">
+        <v>361</v>
+      </c>
+      <c r="T14" t="s">
+        <v>251</v>
+      </c>
+      <c r="U14" t="s">
+        <v>362</v>
+      </c>
+      <c r="V14" t="s">
+        <v>297</v>
+      </c>
+      <c r="W14" t="s">
+        <v>363</v>
+      </c>
       <c r="Y14" s="39"/>
     </row>
     <row r="15" spans="1:25" s="43" customFormat="1" ht="15">
@@ -8346,11 +8368,19 @@
       <c r="K37" s="70" t="s">
         <v>356</v>
       </c>
-      <c r="M37" s="40"/>
-      <c r="N37" s="39"/>
+      <c r="M37" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="N37" s="39" t="s">
+        <v>86</v>
+      </c>
       <c r="O37" s="41"/>
-      <c r="P37" s="41"/>
-      <c r="Q37" s="61"/>
+      <c r="P37" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q37" s="61" t="s">
+        <v>364</v>
+      </c>
       <c r="R37" s="50" t="s">
         <v>218</v>
       </c>
@@ -9451,13 +9481,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -9471,6 +9494,13 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M43">
@@ -9493,7 +9523,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Escaleta MA_06_04_CO revisada y con ajustes para asistente digital
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/MA_06_04_CO Escaleta.xlsx
+++ b/fuentes/contenidos/grado06/guion04/MA_06_04_CO Escaleta.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14860" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="386">
   <si>
     <t>Asignatura</t>
   </si>
@@ -813,9 +813,6 @@
     <t>Recurso M1C-01</t>
   </si>
   <si>
-    <t>Recurso M3A-01</t>
-  </si>
-  <si>
     <t>Recurso M10A-01</t>
   </si>
   <si>
@@ -840,9 +837,6 @@
     <t>Elaborar texto contando la historia de los números amigos y cómo se forman; de la misma manera para los números perfectos. Mostrar ejemplos de dichos números y pedirles que inventen un tipo de número: Números divertidos , por ejemplo. Deberán asignar un criterio para estos números.</t>
   </si>
   <si>
-    <t>Recurso F6-02</t>
-  </si>
-  <si>
     <t>Recurso M5A-01</t>
   </si>
   <si>
@@ -1117,6 +1111,75 @@
   </si>
   <si>
     <t>Enunciados en los cuales se plantean actividades de problemas sencillos de los conceptos de míltuplis, divisores, mcm y mcd</t>
+  </si>
+  <si>
+    <t>Recurso F6B-02</t>
+  </si>
+  <si>
+    <t>Recurso M2C-01</t>
+  </si>
+  <si>
+    <t>Recurso M102AB-01</t>
+  </si>
+  <si>
+    <t>Recurso M102AB-02</t>
+  </si>
+  <si>
+    <t>Recurso M8A-01</t>
+  </si>
+  <si>
+    <t>Recurso M101A-01</t>
+  </si>
+  <si>
+    <t>Recurso M4A-01</t>
+  </si>
+  <si>
+    <t>Recurso M8A-02</t>
+  </si>
+  <si>
+    <t>Recurso M101A-02</t>
+  </si>
+  <si>
+    <t>Recurso M101A-03</t>
+  </si>
+  <si>
+    <t>Recurso M2C-02</t>
+  </si>
+  <si>
+    <t>Recurso M4A-02</t>
+  </si>
+  <si>
+    <t>Recurso M7A-01</t>
+  </si>
+  <si>
+    <t>Recurso M101A-04</t>
+  </si>
+  <si>
+    <t>Recurso M1A-01</t>
+  </si>
+  <si>
+    <t>Recurso M101A-05</t>
+  </si>
+  <si>
+    <t>Recurso M1A-02</t>
+  </si>
+  <si>
+    <t>Recurso M4A-03</t>
+  </si>
+  <si>
+    <t>Recurso M6A-01</t>
+  </si>
+  <si>
+    <t>Recursos adicionales 01</t>
+  </si>
+  <si>
+    <t>Recurso M101A-06</t>
+  </si>
+  <si>
+    <t>RF_01_02_CO</t>
+  </si>
+  <si>
+    <t>Recurso M5A-02</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1202,8 +1265,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1291,6 +1361,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1412,7 +1488,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1479,8 +1555,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1632,9 +1709,6 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1653,34 +1727,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1719,8 +1781,47 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="64">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1759,6 +1860,7 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6377,138 +6479,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G12" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="O20" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" style="67" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="67" customWidth="1"/>
-    <col min="3" max="3" width="35.5" style="67" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="67" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="67" customWidth="1"/>
-    <col min="6" max="6" width="37.1640625" style="67" customWidth="1"/>
-    <col min="7" max="7" width="32.83203125" style="67" customWidth="1"/>
-    <col min="8" max="8" width="36.1640625" style="67" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" style="67" customWidth="1"/>
-    <col min="10" max="10" width="31.33203125" style="67" customWidth="1"/>
-    <col min="11" max="11" width="62.33203125" style="73" customWidth="1"/>
-    <col min="13" max="13" width="27" style="67" customWidth="1"/>
-    <col min="14" max="14" width="29.5" style="67" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" style="67" customWidth="1"/>
-    <col min="16" max="16" width="15.5" style="67" customWidth="1"/>
-    <col min="17" max="17" width="78.6640625" style="67" customWidth="1"/>
-    <col min="18" max="18" width="17.33203125" style="67" customWidth="1"/>
-    <col min="19" max="19" width="28.5" style="68" customWidth="1"/>
-    <col min="20" max="20" width="23.33203125" style="69" customWidth="1"/>
-    <col min="21" max="21" width="24.5" style="68" customWidth="1"/>
-    <col min="22" max="22" width="26.5" style="69" customWidth="1"/>
-    <col min="23" max="23" width="24" style="68" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" style="67"/>
-    <col min="25" max="25" width="26.6640625" style="67" customWidth="1"/>
-    <col min="26" max="16384" width="10.83203125" style="67"/>
+    <col min="1" max="1" width="31.1640625" style="66" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="66" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="66" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="66" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" style="66" customWidth="1"/>
+    <col min="6" max="6" width="37.1640625" style="66" customWidth="1"/>
+    <col min="7" max="7" width="32.83203125" style="66" customWidth="1"/>
+    <col min="8" max="8" width="36.1640625" style="66" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" style="66" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" style="66" customWidth="1"/>
+    <col min="11" max="11" width="62.33203125" style="72" customWidth="1"/>
+    <col min="13" max="13" width="27" style="66" customWidth="1"/>
+    <col min="14" max="14" width="29.5" style="66" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" style="66" customWidth="1"/>
+    <col min="16" max="16" width="15.5" style="66" customWidth="1"/>
+    <col min="17" max="17" width="78.6640625" style="66" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" style="66" customWidth="1"/>
+    <col min="19" max="19" width="28.5" style="67" customWidth="1"/>
+    <col min="20" max="20" width="23.33203125" style="68" customWidth="1"/>
+    <col min="21" max="21" width="24.5" style="67" customWidth="1"/>
+    <col min="22" max="22" width="26.5" style="68" customWidth="1"/>
+    <col min="23" max="23" width="24" style="67" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="66"/>
+    <col min="25" max="25" width="26.6640625" style="66" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="66"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="43" customFormat="1" ht="15">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="89" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="81" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>278</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="75" t="s">
+        <v>201</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>202</v>
+      </c>
+      <c r="K1" s="85" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="83" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="86" t="s">
-        <v>279</v>
-      </c>
-      <c r="F1" s="84" t="s">
-        <v>280</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>281</v>
-      </c>
-      <c r="H1" s="76" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="82" t="s">
-        <v>201</v>
-      </c>
-      <c r="J1" s="76" t="s">
-        <v>202</v>
-      </c>
-      <c r="K1" s="90" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="88" t="s">
-        <v>277</v>
-      </c>
-      <c r="N1" s="76" t="s">
+      <c r="N1" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="92" t="s">
+      <c r="O1" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="74" t="s">
+      <c r="P1" s="88"/>
+      <c r="Q1" s="77" t="s">
         <v>203</v>
       </c>
-      <c r="R1" s="74" t="s">
+      <c r="R1" s="77" t="s">
         <v>204</v>
       </c>
-      <c r="S1" s="78" t="s">
+      <c r="S1" s="91" t="s">
         <v>123</v>
       </c>
-      <c r="T1" s="80" t="s">
+      <c r="T1" s="93" t="s">
         <v>124</v>
       </c>
-      <c r="U1" s="78" t="s">
+      <c r="U1" s="91" t="s">
         <v>125</v>
       </c>
-      <c r="V1" s="80" t="s">
+      <c r="V1" s="93" t="s">
         <v>126</v>
       </c>
-      <c r="W1" s="78" t="s">
+      <c r="W1" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="Y1" s="76" t="s">
+      <c r="Y1" s="73" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="43" customFormat="1" ht="15">
-      <c r="A2" s="87"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="95"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="90"/>
       <c r="D2" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="85"/>
+        <v>274</v>
+      </c>
+      <c r="E2" s="82"/>
+      <c r="F2" s="80"/>
       <c r="G2" s="32"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="91"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="77"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="86"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="74"/>
       <c r="O2" s="30" t="s">
         <v>128</v>
       </c>
       <c r="P2" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="79"/>
-      <c r="Y2" s="77"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="94"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="92"/>
+      <c r="Y2" s="74"/>
     </row>
     <row r="3" spans="1:25" s="43" customFormat="1" ht="79" customHeight="1">
       <c r="A3" s="35" t="s">
@@ -6521,7 +6623,7 @@
         <v>216</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E3" s="35" t="s">
         <v>221</v>
@@ -6531,7 +6633,7 @@
       </c>
       <c r="G3" s="36"/>
       <c r="H3" s="39" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I3" s="38">
         <v>1</v>
@@ -6539,8 +6641,8 @@
       <c r="J3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="70" t="s">
-        <v>286</v>
+      <c r="K3" s="69" t="s">
+        <v>284</v>
       </c>
       <c r="M3" s="40" t="s">
         <v>79</v>
@@ -6549,11 +6651,11 @@
         <v>84</v>
       </c>
       <c r="O3" s="41" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P3" s="41"/>
-      <c r="Q3" s="61" t="s">
-        <v>287</v>
+      <c r="Q3" s="95" t="s">
+        <v>285</v>
       </c>
       <c r="R3" s="44" t="s">
         <v>218</v>
@@ -6577,7 +6679,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="4" spans="1:25" s="43" customFormat="1" ht="42">
       <c r="A4" s="35" t="s">
         <v>76</v>
       </c>
@@ -6588,7 +6690,7 @@
         <v>216</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E4" s="35" t="s">
         <v>221</v>
@@ -6598,7 +6700,7 @@
       </c>
       <c r="G4" s="49"/>
       <c r="H4" s="39" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I4" s="38">
         <v>2</v>
@@ -6606,8 +6708,8 @@
       <c r="J4" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="70" t="s">
-        <v>357</v>
+      <c r="K4" s="96" t="s">
+        <v>355</v>
       </c>
       <c r="M4" s="40" t="s">
         <v>79</v>
@@ -6619,7 +6721,7 @@
         <v>93</v>
       </c>
       <c r="P4" s="41"/>
-      <c r="Q4" s="61" t="s">
+      <c r="Q4" s="95" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="50" t="s">
@@ -6644,7 +6746,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="5" spans="1:25" s="43" customFormat="1" ht="56">
       <c r="A5" s="35" t="s">
         <v>76</v>
       </c>
@@ -6655,7 +6757,7 @@
         <v>216</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>221</v>
@@ -6665,7 +6767,7 @@
       </c>
       <c r="G5" s="48"/>
       <c r="H5" s="42" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I5" s="38">
         <v>3</v>
@@ -6673,8 +6775,8 @@
       <c r="J5" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="70" t="s">
-        <v>323</v>
+      <c r="K5" s="69" t="s">
+        <v>321</v>
       </c>
       <c r="M5" s="40" t="s">
         <v>79</v>
@@ -6686,7 +6788,7 @@
       <c r="P5" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="Q5" s="64" t="s">
+      <c r="Q5" s="98" t="s">
         <v>219</v>
       </c>
       <c r="R5" s="50" t="s">
@@ -6711,7 +6813,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="6" spans="1:25" s="43" customFormat="1" ht="56">
       <c r="A6" s="35" t="s">
         <v>76</v>
       </c>
@@ -6728,35 +6830,51 @@
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
       <c r="H6" s="42" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I6" s="38">
         <v>4</v>
       </c>
       <c r="J6" s="39"/>
-      <c r="K6" s="70" t="s">
-        <v>326</v>
-      </c>
-      <c r="M6" s="40"/>
-      <c r="N6" s="39"/>
+      <c r="K6" s="96" t="s">
+        <v>324</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="39" t="s">
+        <v>86</v>
+      </c>
       <c r="O6" s="41"/>
       <c r="P6" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="Q6" s="65" t="s">
-        <v>283</v>
+      <c r="Q6" s="99" t="s">
+        <v>281</v>
       </c>
       <c r="R6" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="S6" s="45"/>
-      <c r="T6" s="46"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="45"/>
-      <c r="Y6" s="39"/>
-    </row>
-    <row r="7" spans="1:25" s="43" customFormat="1" ht="15">
+      <c r="S6">
+        <v>6</v>
+      </c>
+      <c r="T6" t="s">
+        <v>257</v>
+      </c>
+      <c r="U6" t="s">
+        <v>258</v>
+      </c>
+      <c r="V6" s="103" t="s">
+        <v>271</v>
+      </c>
+      <c r="W6" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y6" s="39" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A7" s="35" t="s">
         <v>76</v>
       </c>
@@ -6767,7 +6885,7 @@
         <v>216</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>221</v>
@@ -6776,8 +6894,8 @@
         <v>212</v>
       </c>
       <c r="G7" s="48"/>
-      <c r="H7" s="42" t="s">
-        <v>288</v>
+      <c r="H7" s="97" t="s">
+        <v>286</v>
       </c>
       <c r="I7" s="38">
         <v>5</v>
@@ -6785,8 +6903,8 @@
       <c r="J7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="70" t="s">
-        <v>324</v>
+      <c r="K7" s="96" t="s">
+        <v>322</v>
       </c>
       <c r="M7" s="40" t="s">
         <v>79</v>
@@ -6802,26 +6920,26 @@
       <c r="R7" s="50" t="s">
         <v>215</v>
       </c>
-      <c r="S7" s="45">
+      <c r="S7" s="101">
         <v>6</v>
       </c>
-      <c r="T7" s="46" t="s">
+      <c r="T7" s="101" t="s">
         <v>257</v>
       </c>
-      <c r="U7" s="45" t="s">
+      <c r="U7" s="101" t="s">
         <v>258</v>
       </c>
-      <c r="V7" s="47" t="s">
-        <v>261</v>
-      </c>
-      <c r="W7" s="45" t="s">
+      <c r="V7" s="102" t="s">
+        <v>368</v>
+      </c>
+      <c r="W7" s="101" t="s">
         <v>260</v>
       </c>
       <c r="Y7" s="39" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="8" spans="1:25" s="43" customFormat="1" ht="42">
       <c r="A8" s="35" t="s">
         <v>76</v>
       </c>
@@ -6850,7 +6968,7 @@
       <c r="J8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="70" t="s">
+      <c r="K8" s="69" t="s">
         <v>224</v>
       </c>
       <c r="M8" s="40" t="s">
@@ -6860,11 +6978,11 @@
         <v>84</v>
       </c>
       <c r="O8" s="41" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P8" s="41"/>
-      <c r="Q8" s="64" t="s">
-        <v>289</v>
+      <c r="Q8" s="98" t="s">
+        <v>287</v>
       </c>
       <c r="R8" s="50" t="s">
         <v>215</v>
@@ -6879,7 +6997,7 @@
         <v>244</v>
       </c>
       <c r="V8" s="47" t="s">
-        <v>247</v>
+        <v>363</v>
       </c>
       <c r="W8" s="45" t="s">
         <v>246</v>
@@ -6915,8 +7033,8 @@
       <c r="J9" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="K9" s="70" t="s">
-        <v>358</v>
+      <c r="K9" s="69" t="s">
+        <v>356</v>
       </c>
       <c r="M9" s="40" t="s">
         <v>79</v>
@@ -6953,7 +7071,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="10" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A10" s="35" t="s">
         <v>76</v>
       </c>
@@ -6970,14 +7088,14 @@
       <c r="F10" s="48"/>
       <c r="G10" s="49"/>
       <c r="H10" s="55" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="I10" s="38">
         <v>8</v>
       </c>
       <c r="J10" s="42"/>
-      <c r="K10" s="70" t="s">
-        <v>327</v>
+      <c r="K10" s="96" t="s">
+        <v>325</v>
       </c>
       <c r="M10" s="40"/>
       <c r="N10" s="39"/>
@@ -6986,19 +7104,29 @@
         <v>106</v>
       </c>
       <c r="Q10" s="61" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="R10" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="S10" s="45"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="45"/>
-      <c r="V10" s="47"/>
-      <c r="W10" s="45"/>
+      <c r="S10" s="101">
+        <v>6</v>
+      </c>
+      <c r="T10" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U10" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V10" s="102" t="s">
+        <v>367</v>
+      </c>
+      <c r="W10" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y10" s="39"/>
     </row>
-    <row r="11" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="11" spans="1:25" s="43" customFormat="1" ht="42">
       <c r="A11" s="35" t="s">
         <v>76</v>
       </c>
@@ -7017,7 +7145,7 @@
       </c>
       <c r="G11" s="49"/>
       <c r="H11" s="39" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I11" s="38">
         <v>9</v>
@@ -7025,8 +7153,8 @@
       <c r="J11" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="K11" s="70" t="s">
-        <v>325</v>
+      <c r="K11" s="96" t="s">
+        <v>323</v>
       </c>
       <c r="M11" s="40" t="s">
         <v>79</v>
@@ -7038,8 +7166,8 @@
       <c r="P11" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="Q11" s="61" t="s">
-        <v>294</v>
+      <c r="Q11" s="95" t="s">
+        <v>292</v>
       </c>
       <c r="R11" s="50" t="s">
         <v>215</v>
@@ -7054,7 +7182,7 @@
         <v>258</v>
       </c>
       <c r="V11" s="47" t="s">
-        <v>263</v>
+        <v>364</v>
       </c>
       <c r="W11" s="45" t="s">
         <v>260</v>
@@ -7090,8 +7218,8 @@
       <c r="J12" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="K12" s="70" t="s">
-        <v>328</v>
+      <c r="K12" s="69" t="s">
+        <v>326</v>
       </c>
       <c r="M12" s="40" t="s">
         <v>79</v>
@@ -7119,7 +7247,7 @@
         <v>258</v>
       </c>
       <c r="V12" s="47" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="W12" s="45" t="s">
         <v>260</v>
@@ -7155,8 +7283,8 @@
       <c r="J13" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="K13" s="70" t="s">
-        <v>329</v>
+      <c r="K13" s="69" t="s">
+        <v>327</v>
       </c>
       <c r="M13" s="40" t="s">
         <v>79</v>
@@ -7184,7 +7312,7 @@
         <v>258</v>
       </c>
       <c r="V13" s="47" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W13" s="45" t="s">
         <v>260</v>
@@ -7193,7 +7321,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="14" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A14" s="35" t="s">
         <v>76</v>
       </c>
@@ -7209,15 +7337,15 @@
       </c>
       <c r="F14" s="48"/>
       <c r="G14" s="49"/>
-      <c r="H14" s="39" t="s">
-        <v>297</v>
+      <c r="H14" s="100" t="s">
+        <v>295</v>
       </c>
       <c r="I14" s="38">
         <v>12</v>
       </c>
       <c r="J14" s="42"/>
-      <c r="K14" s="70" t="s">
-        <v>330</v>
+      <c r="K14" s="69" t="s">
+        <v>328</v>
       </c>
       <c r="M14" s="40"/>
       <c r="N14" s="39"/>
@@ -7227,26 +7355,26 @@
         <v>16</v>
       </c>
       <c r="R14" s="50" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="S14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="T14" t="s">
         <v>251</v>
       </c>
       <c r="U14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="V14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="W14" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="Y14" s="39"/>
     </row>
-    <row r="15" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="15" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A15" s="35" t="s">
         <v>76</v>
       </c>
@@ -7264,15 +7392,15 @@
         <v>212</v>
       </c>
       <c r="G15" s="49"/>
-      <c r="H15" s="39" t="s">
-        <v>295</v>
+      <c r="H15" s="100" t="s">
+        <v>293</v>
       </c>
       <c r="I15" s="38">
         <v>13</v>
       </c>
       <c r="J15" s="42"/>
-      <c r="K15" s="70" t="s">
-        <v>335</v>
+      <c r="K15" s="69" t="s">
+        <v>333</v>
       </c>
       <c r="M15" s="40"/>
       <c r="N15" s="39"/>
@@ -7281,16 +7409,26 @@
         <v>120</v>
       </c>
       <c r="Q15" s="61" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="R15" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S15" s="45"/>
-      <c r="T15" s="46"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="47"/>
-      <c r="W15" s="45"/>
+        <v>352</v>
+      </c>
+      <c r="S15" s="101">
+        <v>6</v>
+      </c>
+      <c r="T15" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U15" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V15" s="102" t="s">
+        <v>371</v>
+      </c>
+      <c r="W15" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y15" s="39"/>
     </row>
     <row r="16" spans="1:25" s="43" customFormat="1" ht="15">
@@ -7318,8 +7456,8 @@
       <c r="J16" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="K16" s="70" t="s">
-        <v>266</v>
+      <c r="K16" s="69" t="s">
+        <v>265</v>
       </c>
       <c r="M16" s="40" t="s">
         <v>80</v>
@@ -7379,8 +7517,8 @@
       <c r="J17" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="K17" s="70" t="s">
-        <v>331</v>
+      <c r="K17" s="69" t="s">
+        <v>329</v>
       </c>
       <c r="M17" s="40" t="s">
         <v>80</v>
@@ -7394,7 +7532,7 @@
         <v>255</v>
       </c>
       <c r="R17" s="50" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="S17" s="57" t="s">
         <v>250</v>
@@ -7440,8 +7578,8 @@
       <c r="J18" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="K18" s="70" t="s">
-        <v>332</v>
+      <c r="K18" s="69" t="s">
+        <v>330</v>
       </c>
       <c r="M18" s="40" t="s">
         <v>79</v>
@@ -7466,7 +7604,7 @@
         <v>258</v>
       </c>
       <c r="U18" s="58" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="V18" s="46" t="s">
         <v>260</v>
@@ -7493,14 +7631,14 @@
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
       <c r="H19" s="39" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I19" s="38">
         <v>17</v>
       </c>
       <c r="J19" s="42"/>
-      <c r="K19" s="70" t="s">
-        <v>299</v>
+      <c r="K19" s="69" t="s">
+        <v>297</v>
       </c>
       <c r="M19" s="40"/>
       <c r="N19" s="39"/>
@@ -7509,19 +7647,29 @@
         <v>141</v>
       </c>
       <c r="Q19" s="61" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="R19" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="S19" s="45"/>
-      <c r="T19" s="46"/>
-      <c r="U19" s="58"/>
-      <c r="V19" s="46"/>
-      <c r="W19" s="53"/>
+      <c r="S19">
+        <v>6</v>
+      </c>
+      <c r="T19" t="s">
+        <v>257</v>
+      </c>
+      <c r="U19" t="s">
+        <v>258</v>
+      </c>
+      <c r="V19" s="103" t="s">
+        <v>369</v>
+      </c>
+      <c r="W19" t="s">
+        <v>260</v>
+      </c>
       <c r="Y19" s="39"/>
     </row>
-    <row r="20" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="20" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A20" s="35" t="s">
         <v>76</v>
       </c>
@@ -7537,15 +7685,15 @@
       </c>
       <c r="F20" s="48"/>
       <c r="G20" s="49"/>
-      <c r="H20" s="39" t="s">
-        <v>301</v>
+      <c r="H20" s="100" t="s">
+        <v>299</v>
       </c>
       <c r="I20" s="38">
         <v>18</v>
       </c>
       <c r="J20" s="42"/>
-      <c r="K20" s="70" t="s">
-        <v>333</v>
+      <c r="K20" s="96" t="s">
+        <v>331</v>
       </c>
       <c r="M20" s="40"/>
       <c r="N20" s="39"/>
@@ -7554,19 +7702,29 @@
         <v>106</v>
       </c>
       <c r="Q20" s="61" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="R20" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="S20" s="45"/>
-      <c r="T20" s="46"/>
-      <c r="U20" s="58"/>
-      <c r="V20" s="46"/>
-      <c r="W20" s="53"/>
+      <c r="S20" s="101">
+        <v>6</v>
+      </c>
+      <c r="T20" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U20" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V20" s="102" t="s">
+        <v>370</v>
+      </c>
+      <c r="W20" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y20" s="39"/>
     </row>
-    <row r="21" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="21" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A21" s="35" t="s">
         <v>76</v>
       </c>
@@ -7584,15 +7742,15 @@
         <v>212</v>
       </c>
       <c r="G21" s="49"/>
-      <c r="H21" s="39" t="s">
-        <v>334</v>
+      <c r="H21" s="100" t="s">
+        <v>332</v>
       </c>
       <c r="I21" s="38">
         <v>19</v>
       </c>
       <c r="J21" s="42"/>
-      <c r="K21" s="70" t="s">
-        <v>336</v>
+      <c r="K21" s="69" t="s">
+        <v>334</v>
       </c>
       <c r="M21" s="40"/>
       <c r="N21" s="39"/>
@@ -7602,13 +7760,23 @@
       </c>
       <c r="Q21" s="61"/>
       <c r="R21" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S21" s="45"/>
-      <c r="T21" s="46"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="46"/>
-      <c r="W21" s="53"/>
+        <v>352</v>
+      </c>
+      <c r="S21" s="101">
+        <v>6</v>
+      </c>
+      <c r="T21" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U21" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V21" s="102" t="s">
+        <v>372</v>
+      </c>
+      <c r="W21" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y21" s="39"/>
     </row>
     <row r="22" spans="1:25" s="43" customFormat="1" ht="15">
@@ -7638,7 +7806,7 @@
       <c r="J22" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="K22" s="70" t="s">
+      <c r="K22" s="69" t="s">
         <v>236</v>
       </c>
       <c r="M22" s="40" t="s">
@@ -7651,8 +7819,8 @@
         <v>101</v>
       </c>
       <c r="P22" s="41"/>
-      <c r="Q22" s="66" t="s">
-        <v>303</v>
+      <c r="Q22" s="65" t="s">
+        <v>301</v>
       </c>
       <c r="R22" s="50" t="s">
         <v>218</v>
@@ -7664,7 +7832,7 @@
         <v>244</v>
       </c>
       <c r="U22" s="58" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="V22" s="46" t="s">
         <v>246</v>
@@ -7693,7 +7861,7 @@
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="39" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I23" s="38">
         <v>21</v>
@@ -7701,7 +7869,7 @@
       <c r="J23" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="K23" s="70" t="s">
+      <c r="K23" s="69" t="s">
         <v>237</v>
       </c>
       <c r="M23" s="40" t="s">
@@ -7715,7 +7883,7 @@
         <v>109</v>
       </c>
       <c r="Q23" s="61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="R23" s="50" t="s">
         <v>215</v>
@@ -7730,7 +7898,7 @@
         <v>252</v>
       </c>
       <c r="V23" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="W23" s="45" t="s">
         <v>253</v>
@@ -7739,7 +7907,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="24" spans="1:25" s="43" customFormat="1" ht="28">
       <c r="A24" s="35" t="s">
         <v>76</v>
       </c>
@@ -7756,14 +7924,14 @@
       <c r="F24" s="48"/>
       <c r="G24" s="49"/>
       <c r="H24" s="39" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I24" s="38">
         <v>22</v>
       </c>
       <c r="J24" s="42"/>
-      <c r="K24" s="70" t="s">
-        <v>309</v>
+      <c r="K24" s="69" t="s">
+        <v>307</v>
       </c>
       <c r="M24" s="40"/>
       <c r="N24" s="39"/>
@@ -7771,17 +7939,27 @@
       <c r="P24" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="Q24" s="61" t="s">
-        <v>306</v>
+      <c r="Q24" s="95" t="s">
+        <v>304</v>
       </c>
       <c r="R24" s="50" t="s">
         <v>215</v>
       </c>
-      <c r="S24" s="45"/>
-      <c r="T24" s="46"/>
-      <c r="U24" s="45"/>
-      <c r="V24" s="46"/>
-      <c r="W24" s="45"/>
+      <c r="S24" s="101">
+        <v>6</v>
+      </c>
+      <c r="T24" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U24" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V24" s="102" t="s">
+        <v>373</v>
+      </c>
+      <c r="W24" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y24" s="39"/>
     </row>
     <row r="25" spans="1:25" s="43" customFormat="1" ht="15">
@@ -7811,8 +7989,8 @@
       <c r="J25" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="K25" s="70" t="s">
-        <v>359</v>
+      <c r="K25" s="69" t="s">
+        <v>357</v>
       </c>
       <c r="M25" s="40" t="s">
         <v>79</v>
@@ -7839,7 +8017,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="26" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="26" spans="1:25" s="43" customFormat="1" ht="28">
       <c r="A26" s="35" t="s">
         <v>76</v>
       </c>
@@ -7856,14 +8034,14 @@
       <c r="F26" s="48"/>
       <c r="G26" s="49"/>
       <c r="H26" s="39" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I26" s="38">
         <v>24</v>
       </c>
       <c r="J26" s="42"/>
-      <c r="K26" s="70" t="s">
-        <v>311</v>
+      <c r="K26" s="69" t="s">
+        <v>309</v>
       </c>
       <c r="M26" s="40" t="s">
         <v>79</v>
@@ -7873,17 +8051,27 @@
       <c r="P26" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="Q26" s="51" t="s">
-        <v>312</v>
+      <c r="Q26" s="104" t="s">
+        <v>310</v>
       </c>
       <c r="R26" s="50" t="s">
         <v>215</v>
       </c>
-      <c r="S26" s="59"/>
-      <c r="T26" s="60"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="60"/>
-      <c r="W26" s="53"/>
+      <c r="S26" s="101">
+        <v>6</v>
+      </c>
+      <c r="T26" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U26" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V26" s="102" t="s">
+        <v>374</v>
+      </c>
+      <c r="W26" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y26" s="39"/>
     </row>
     <row r="27" spans="1:25" s="43" customFormat="1" ht="15">
@@ -7903,14 +8091,14 @@
       <c r="F27" s="48"/>
       <c r="G27" s="49"/>
       <c r="H27" s="39" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I27" s="38">
         <v>25</v>
       </c>
       <c r="J27" s="42"/>
-      <c r="K27" s="70" t="s">
-        <v>339</v>
+      <c r="K27" s="69" t="s">
+        <v>337</v>
       </c>
       <c r="M27" s="40"/>
       <c r="N27" s="39"/>
@@ -7919,19 +8107,29 @@
         <v>105</v>
       </c>
       <c r="Q27" s="51" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="R27" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="S27" s="59"/>
-      <c r="T27" s="60"/>
-      <c r="U27" s="59"/>
-      <c r="V27" s="60"/>
-      <c r="W27" s="53"/>
+      <c r="S27" s="101">
+        <v>6</v>
+      </c>
+      <c r="T27" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U27" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V27" s="102" t="s">
+        <v>375</v>
+      </c>
+      <c r="W27" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y27" s="39"/>
     </row>
-    <row r="28" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="28" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A28" s="35"/>
       <c r="B28" s="36"/>
       <c r="C28" s="37"/>
@@ -7943,15 +8141,15 @@
         <v>212</v>
       </c>
       <c r="G28" s="49"/>
-      <c r="H28" s="39" t="s">
-        <v>348</v>
+      <c r="H28" s="100" t="s">
+        <v>346</v>
       </c>
       <c r="I28" s="38">
         <v>26</v>
       </c>
       <c r="J28" s="42"/>
-      <c r="K28" s="70" t="s">
-        <v>355</v>
+      <c r="K28" s="69" t="s">
+        <v>353</v>
       </c>
       <c r="M28" s="40"/>
       <c r="N28" s="39"/>
@@ -7961,13 +8159,23 @@
       </c>
       <c r="Q28" s="51"/>
       <c r="R28" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S28" s="59"/>
-      <c r="T28" s="60"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="60"/>
-      <c r="W28" s="53"/>
+        <v>352</v>
+      </c>
+      <c r="S28" s="101">
+        <v>6</v>
+      </c>
+      <c r="T28" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U28" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V28" s="102" t="s">
+        <v>376</v>
+      </c>
+      <c r="W28" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y28" s="39"/>
     </row>
     <row r="29" spans="1:25" s="43" customFormat="1" ht="15">
@@ -7982,19 +8190,19 @@
       </c>
       <c r="D29" s="37"/>
       <c r="E29" s="52" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F29" s="48"/>
       <c r="G29" s="49"/>
       <c r="H29" s="39" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I29" s="38">
         <v>27</v>
       </c>
       <c r="J29" s="42"/>
-      <c r="K29" s="70" t="s">
-        <v>338</v>
+      <c r="K29" s="69" t="s">
+        <v>336</v>
       </c>
       <c r="M29" s="40"/>
       <c r="N29" s="39"/>
@@ -8004,16 +8212,26 @@
       </c>
       <c r="Q29" s="51"/>
       <c r="R29" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S29" s="59"/>
-      <c r="T29" s="60"/>
-      <c r="U29" s="59"/>
-      <c r="V29" s="60"/>
-      <c r="W29" s="53"/>
+        <v>352</v>
+      </c>
+      <c r="S29" s="101">
+        <v>6</v>
+      </c>
+      <c r="T29" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U29" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V29" s="102" t="s">
+        <v>377</v>
+      </c>
+      <c r="W29" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y29" s="39"/>
     </row>
-    <row r="30" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="30" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A30" s="35" t="s">
         <v>76</v>
       </c>
@@ -8025,21 +8243,21 @@
       </c>
       <c r="D30" s="37"/>
       <c r="E30" s="52" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>212</v>
       </c>
       <c r="G30" s="49"/>
-      <c r="H30" s="39" t="s">
-        <v>321</v>
+      <c r="H30" s="100" t="s">
+        <v>319</v>
       </c>
       <c r="I30" s="38">
         <v>28</v>
       </c>
       <c r="J30" s="42"/>
-      <c r="K30" s="70" t="s">
-        <v>337</v>
+      <c r="K30" s="69" t="s">
+        <v>335</v>
       </c>
       <c r="M30" s="40"/>
       <c r="N30" s="39"/>
@@ -8049,13 +8267,23 @@
       </c>
       <c r="Q30" s="51"/>
       <c r="R30" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S30" s="59"/>
-      <c r="T30" s="60"/>
-      <c r="U30" s="59"/>
-      <c r="V30" s="60"/>
-      <c r="W30" s="53"/>
+        <v>352</v>
+      </c>
+      <c r="S30" s="101">
+        <v>6</v>
+      </c>
+      <c r="T30" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U30" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V30" s="102" t="s">
+        <v>378</v>
+      </c>
+      <c r="W30" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y30" s="39"/>
     </row>
     <row r="31" spans="1:25" s="43" customFormat="1" ht="15">
@@ -8070,19 +8298,19 @@
       </c>
       <c r="D31" s="37"/>
       <c r="E31" s="52" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F31" s="48"/>
       <c r="G31" s="49"/>
       <c r="H31" s="39" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I31" s="38">
         <v>29</v>
       </c>
       <c r="J31" s="42"/>
-      <c r="K31" s="70" t="s">
-        <v>340</v>
+      <c r="K31" s="69" t="s">
+        <v>338</v>
       </c>
       <c r="M31" s="40"/>
       <c r="N31" s="39"/>
@@ -8092,16 +8320,26 @@
       </c>
       <c r="Q31" s="51"/>
       <c r="R31" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S31" s="59"/>
-      <c r="T31" s="60"/>
-      <c r="U31" s="59"/>
-      <c r="V31" s="60"/>
-      <c r="W31" s="53"/>
+        <v>352</v>
+      </c>
+      <c r="S31" s="101">
+        <v>6</v>
+      </c>
+      <c r="T31" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U31" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V31" s="102" t="s">
+        <v>379</v>
+      </c>
+      <c r="W31" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y31" s="39"/>
     </row>
-    <row r="32" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="32" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A32" s="35" t="s">
         <v>76</v>
       </c>
@@ -8113,19 +8351,19 @@
       </c>
       <c r="D32" s="37"/>
       <c r="E32" s="52" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F32" s="48"/>
       <c r="G32" s="49"/>
-      <c r="H32" s="39" t="s">
-        <v>341</v>
+      <c r="H32" s="100" t="s">
+        <v>339</v>
       </c>
       <c r="I32" s="38">
         <v>30</v>
       </c>
       <c r="J32" s="42"/>
-      <c r="K32" s="70" t="s">
-        <v>342</v>
+      <c r="K32" s="69" t="s">
+        <v>340</v>
       </c>
       <c r="M32" s="40"/>
       <c r="N32" s="39"/>
@@ -8134,16 +8372,26 @@
         <v>141</v>
       </c>
       <c r="Q32" s="51" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R32" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S32" s="59"/>
-      <c r="T32" s="60"/>
-      <c r="U32" s="59"/>
-      <c r="V32" s="60"/>
-      <c r="W32" s="53"/>
+        <v>352</v>
+      </c>
+      <c r="S32" s="101">
+        <v>6</v>
+      </c>
+      <c r="T32" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U32" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V32" s="102" t="s">
+        <v>380</v>
+      </c>
+      <c r="W32" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y32" s="39"/>
     </row>
     <row r="33" spans="1:25" s="43" customFormat="1" ht="15">
@@ -8158,19 +8406,19 @@
       </c>
       <c r="D33" s="37"/>
       <c r="E33" s="52" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F33" s="48"/>
       <c r="G33" s="49"/>
       <c r="H33" s="39" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I33" s="38">
         <v>31</v>
       </c>
       <c r="J33" s="42"/>
-      <c r="K33" s="70" t="s">
-        <v>360</v>
+      <c r="K33" s="69" t="s">
+        <v>358</v>
       </c>
       <c r="M33" s="40"/>
       <c r="N33" s="39"/>
@@ -8179,10 +8427,10 @@
         <v>152</v>
       </c>
       <c r="Q33" s="51" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="R33" s="50" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="S33" s="59"/>
       <c r="T33" s="60"/>
@@ -8203,19 +8451,19 @@
       </c>
       <c r="D34" s="37"/>
       <c r="E34" s="52" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F34" s="48"/>
       <c r="G34" s="49"/>
       <c r="H34" s="39" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I34" s="38">
         <v>32</v>
       </c>
       <c r="J34" s="42"/>
-      <c r="K34" s="70" t="s">
-        <v>343</v>
+      <c r="K34" s="69" t="s">
+        <v>341</v>
       </c>
       <c r="M34" s="40"/>
       <c r="N34" s="39"/>
@@ -8224,19 +8472,29 @@
         <v>103</v>
       </c>
       <c r="Q34" s="51" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R34" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S34" s="59"/>
-      <c r="T34" s="60"/>
-      <c r="U34" s="59"/>
-      <c r="V34" s="60"/>
-      <c r="W34" s="53"/>
+        <v>352</v>
+      </c>
+      <c r="S34" s="101">
+        <v>6</v>
+      </c>
+      <c r="T34" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U34" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V34" s="102" t="s">
+        <v>381</v>
+      </c>
+      <c r="W34" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y34" s="39"/>
     </row>
-    <row r="35" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="35" spans="1:25" s="43" customFormat="1" ht="30">
       <c r="A35" s="35" t="s">
         <v>76</v>
       </c>
@@ -8248,21 +8506,21 @@
       </c>
       <c r="D35" s="37"/>
       <c r="E35" s="52" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>212</v>
       </c>
       <c r="G35" s="49"/>
-      <c r="H35" s="39" t="s">
-        <v>322</v>
+      <c r="H35" s="100" t="s">
+        <v>320</v>
       </c>
       <c r="I35" s="38">
         <v>33</v>
       </c>
       <c r="J35" s="42"/>
-      <c r="K35" s="70" t="s">
-        <v>344</v>
+      <c r="K35" s="69" t="s">
+        <v>342</v>
       </c>
       <c r="M35" s="40"/>
       <c r="N35" s="39"/>
@@ -8272,16 +8530,26 @@
       </c>
       <c r="Q35" s="51"/>
       <c r="R35" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S35" s="59"/>
-      <c r="T35" s="60"/>
-      <c r="U35" s="59"/>
-      <c r="V35" s="60"/>
-      <c r="W35" s="53"/>
+        <v>352</v>
+      </c>
+      <c r="S35" s="101">
+        <v>6</v>
+      </c>
+      <c r="T35" s="101" t="s">
+        <v>243</v>
+      </c>
+      <c r="U35" s="105" t="s">
+        <v>382</v>
+      </c>
+      <c r="V35" s="102" t="s">
+        <v>383</v>
+      </c>
+      <c r="W35" s="105" t="s">
+        <v>384</v>
+      </c>
       <c r="Y35" s="39"/>
     </row>
-    <row r="36" spans="1:25" s="43" customFormat="1" ht="15">
+    <row r="36" spans="1:25" s="43" customFormat="1" ht="42">
       <c r="A36" s="35" t="s">
         <v>76</v>
       </c>
@@ -8293,14 +8561,14 @@
       </c>
       <c r="D36" s="37"/>
       <c r="E36" s="52" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F36" s="48" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G36" s="49"/>
-      <c r="H36" s="39" t="s">
-        <v>270</v>
+      <c r="H36" s="100" t="s">
+        <v>269</v>
       </c>
       <c r="I36" s="38">
         <v>34</v>
@@ -8308,8 +8576,8 @@
       <c r="J36" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="K36" s="70" t="s">
-        <v>274</v>
+      <c r="K36" s="96" t="s">
+        <v>272</v>
       </c>
       <c r="M36" s="40" t="s">
         <v>79</v>
@@ -8321,26 +8589,26 @@
       <c r="P36" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="Q36" s="61" t="s">
-        <v>271</v>
+      <c r="Q36" s="95" t="s">
+        <v>270</v>
       </c>
       <c r="R36" s="50" t="s">
-        <v>354</v>
-      </c>
-      <c r="S36" s="45">
+        <v>352</v>
+      </c>
+      <c r="S36" s="101">
         <v>6</v>
       </c>
-      <c r="T36" s="46" t="s">
-        <v>243</v>
-      </c>
-      <c r="U36" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="V36" s="47" t="s">
-        <v>272</v>
-      </c>
-      <c r="W36" s="45" t="s">
-        <v>246</v>
+      <c r="T36" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U36" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V36" s="102" t="s">
+        <v>365</v>
+      </c>
+      <c r="W36" s="101" t="s">
+        <v>260</v>
       </c>
       <c r="Y36" s="39" t="s">
         <v>208</v>
@@ -8352,21 +8620,21 @@
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
       <c r="E37" s="52" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F37" s="48" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G37" s="49"/>
       <c r="H37" s="39" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I37" s="38">
         <v>35</v>
       </c>
       <c r="J37" s="42"/>
-      <c r="K37" s="70" t="s">
-        <v>356</v>
+      <c r="K37" s="69" t="s">
+        <v>354</v>
       </c>
       <c r="M37" s="40" t="s">
         <v>79</v>
@@ -8379,16 +8647,26 @@
         <v>122</v>
       </c>
       <c r="Q37" s="61" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="R37" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="S37" s="45"/>
-      <c r="T37" s="46"/>
-      <c r="U37" s="45"/>
-      <c r="V37" s="47"/>
-      <c r="W37" s="45"/>
+      <c r="S37">
+        <v>6</v>
+      </c>
+      <c r="T37" t="s">
+        <v>257</v>
+      </c>
+      <c r="U37" t="s">
+        <v>258</v>
+      </c>
+      <c r="V37" s="103" t="s">
+        <v>366</v>
+      </c>
+      <c r="W37" t="s">
+        <v>260</v>
+      </c>
       <c r="Y37" s="39"/>
     </row>
     <row r="38" spans="1:25" s="43" customFormat="1" ht="15">
@@ -8403,7 +8681,7 @@
       </c>
       <c r="D38" s="37"/>
       <c r="E38" s="52" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>14</v>
@@ -8416,8 +8694,8 @@
         <v>36</v>
       </c>
       <c r="J38" s="42"/>
-      <c r="K38" s="70" t="s">
-        <v>345</v>
+      <c r="K38" s="69" t="s">
+        <v>343</v>
       </c>
       <c r="M38" s="40" t="s">
         <v>79</v>
@@ -8429,7 +8707,7 @@
       <c r="P38" s="41"/>
       <c r="Q38" s="51"/>
       <c r="R38" s="50" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="S38" s="53"/>
       <c r="T38" s="54"/>
@@ -8452,7 +8730,7 @@
       </c>
       <c r="D39" s="37"/>
       <c r="E39" s="52" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>242</v>
@@ -8467,8 +8745,8 @@
       <c r="J39" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="K39" s="70" t="s">
-        <v>346</v>
+      <c r="K39" s="69" t="s">
+        <v>344</v>
       </c>
       <c r="M39" s="40" t="s">
         <v>79</v>
@@ -8482,7 +8760,7 @@
       </c>
       <c r="Q39" s="51"/>
       <c r="R39" s="50" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="S39" s="45">
         <v>6</v>
@@ -8494,7 +8772,7 @@
         <v>258</v>
       </c>
       <c r="V39" s="47" t="s">
-        <v>273</v>
+        <v>385</v>
       </c>
       <c r="W39" s="45" t="s">
         <v>260</v>
@@ -8515,7 +8793,7 @@
       </c>
       <c r="D40" s="37"/>
       <c r="E40" s="52" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F40" s="48"/>
       <c r="G40" s="48"/>
@@ -8524,7 +8802,7 @@
         <v>38</v>
       </c>
       <c r="J40" s="42"/>
-      <c r="K40" s="71"/>
+      <c r="K40" s="70"/>
       <c r="M40" s="40"/>
       <c r="N40" s="39"/>
       <c r="O40" s="41"/>
@@ -8535,11 +8813,21 @@
       <c r="R40" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="S40" s="53"/>
-      <c r="T40" s="54"/>
-      <c r="U40" s="53"/>
-      <c r="V40" s="54"/>
-      <c r="W40" s="53"/>
+      <c r="S40" s="101">
+        <v>6</v>
+      </c>
+      <c r="T40" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="U40" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="V40" s="102" t="s">
+        <v>261</v>
+      </c>
+      <c r="W40" s="101" t="s">
+        <v>260</v>
+      </c>
       <c r="Y40" s="39"/>
     </row>
     <row r="41" spans="1:25" s="43" customFormat="1" ht="15">
@@ -8553,7 +8841,7 @@
       <c r="H41" s="42"/>
       <c r="I41" s="62"/>
       <c r="J41" s="42"/>
-      <c r="K41" s="71"/>
+      <c r="K41" s="70"/>
       <c r="M41" s="40"/>
       <c r="N41" s="39"/>
       <c r="O41" s="41"/>
@@ -8578,7 +8866,7 @@
       <c r="H42" s="42"/>
       <c r="I42" s="62"/>
       <c r="J42" s="42"/>
-      <c r="K42" s="71"/>
+      <c r="K42" s="70"/>
       <c r="M42" s="40"/>
       <c r="N42" s="39"/>
       <c r="O42" s="41"/>
@@ -8603,7 +8891,7 @@
       <c r="H43" s="42"/>
       <c r="I43" s="62"/>
       <c r="J43" s="42"/>
-      <c r="K43" s="71"/>
+      <c r="K43" s="70"/>
       <c r="M43" s="40"/>
       <c r="N43" s="39"/>
       <c r="O43" s="41"/>
@@ -8618,7 +8906,7 @@
       <c r="Y43" s="39"/>
     </row>
     <row r="44" spans="1:25" s="43" customFormat="1">
-      <c r="K44" s="72"/>
+      <c r="K44" s="71"/>
       <c r="S44" s="45"/>
       <c r="T44" s="46"/>
       <c r="U44" s="45"/>
@@ -8641,7 +8929,7 @@
       <c r="H45" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="K45" s="72"/>
+      <c r="K45" s="71"/>
       <c r="S45" s="45"/>
       <c r="T45" s="46"/>
       <c r="U45" s="45"/>
@@ -8649,838 +8937,845 @@
       <c r="W45" s="45"/>
     </row>
     <row r="46" spans="1:25">
-      <c r="A46" s="67" t="s">
+      <c r="A46" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="67" t="s">
+      <c r="C46" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="E46" s="67" t="s">
+      <c r="E46" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="L46" s="67"/>
+      <c r="L46" s="66"/>
     </row>
     <row r="47" spans="1:25">
-      <c r="A47" s="67" t="s">
+      <c r="A47" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="67" t="s">
+      <c r="C47" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="67" t="s">
+      <c r="E47" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="F47" s="67" t="s">
+      <c r="F47" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="H47" s="67" t="s">
+      <c r="H47" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="K47" s="73" t="s">
+      <c r="K47" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="L47" s="67"/>
-      <c r="M47" s="67" t="s">
+      <c r="L47" s="66"/>
+      <c r="M47" s="66" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:25">
-      <c r="A48" s="67" t="s">
+      <c r="A48" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="L48" s="67"/>
+      <c r="L48" s="66"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="67" t="s">
+      <c r="A49" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="L49" s="67"/>
+      <c r="L49" s="66"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="67" t="s">
+      <c r="A50" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="L50" s="67"/>
+      <c r="L50" s="66"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="67" t="s">
+      <c r="A51" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="F51" s="67" t="s">
+      <c r="F51" s="66" t="s">
         <v>206</v>
       </c>
-      <c r="L51" s="67"/>
+      <c r="L51" s="66"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="67" t="s">
+      <c r="A52" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="F52" s="67" t="s">
+      <c r="F52" s="66" t="s">
         <v>207</v>
       </c>
-      <c r="L52" s="67"/>
+      <c r="L52" s="66"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="67" t="s">
+      <c r="A53" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="F53" s="67" t="s">
+      <c r="F53" s="66" t="s">
         <v>208</v>
       </c>
-      <c r="L53" s="67"/>
+      <c r="L53" s="66"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="A54" s="67" t="s">
+      <c r="A54" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="F54" s="67" t="s">
+      <c r="F54" s="66" t="s">
         <v>209</v>
       </c>
-      <c r="L54" s="67"/>
+      <c r="L54" s="66"/>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55" s="67" t="s">
+      <c r="A55" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="F55" s="67" t="s">
+      <c r="F55" s="66" t="s">
         <v>210</v>
       </c>
-      <c r="L55" s="67"/>
+      <c r="L55" s="66"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="67" t="s">
+      <c r="A56" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="L56" s="67"/>
+      <c r="L56" s="66"/>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="67" t="s">
+      <c r="A57" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="L57" s="67"/>
+      <c r="L57" s="66"/>
     </row>
     <row r="58" spans="1:12">
-      <c r="A58" s="67" t="s">
+      <c r="A58" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="L58" s="67"/>
+      <c r="L58" s="66"/>
     </row>
     <row r="59" spans="1:12">
-      <c r="A59" s="67" t="s">
+      <c r="A59" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="L59" s="67"/>
+      <c r="L59" s="66"/>
     </row>
     <row r="60" spans="1:12">
-      <c r="A60" s="67" t="s">
+      <c r="A60" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="L60" s="67"/>
+      <c r="L60" s="66"/>
     </row>
     <row r="61" spans="1:12">
-      <c r="A61" s="67" t="s">
+      <c r="A61" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="L61" s="67"/>
+      <c r="L61" s="66"/>
     </row>
     <row r="62" spans="1:12">
-      <c r="L62" s="67"/>
+      <c r="L62" s="66"/>
     </row>
     <row r="63" spans="1:12">
-      <c r="A63" s="67" t="s">
+      <c r="A63" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="L63" s="67"/>
+      <c r="L63" s="66"/>
     </row>
     <row r="64" spans="1:12">
-      <c r="L64" s="67"/>
+      <c r="L64" s="66"/>
     </row>
     <row r="65" spans="12:12">
-      <c r="L65" s="67"/>
+      <c r="L65" s="66"/>
     </row>
     <row r="66" spans="12:12">
-      <c r="L66" s="67"/>
+      <c r="L66" s="66"/>
     </row>
     <row r="67" spans="12:12">
-      <c r="L67" s="67"/>
+      <c r="L67" s="66"/>
     </row>
     <row r="68" spans="12:12">
-      <c r="L68" s="67"/>
+      <c r="L68" s="66"/>
     </row>
     <row r="69" spans="12:12">
-      <c r="L69" s="67"/>
+      <c r="L69" s="66"/>
     </row>
     <row r="70" spans="12:12">
-      <c r="L70" s="67"/>
+      <c r="L70" s="66"/>
     </row>
     <row r="71" spans="12:12">
-      <c r="L71" s="67"/>
+      <c r="L71" s="66"/>
     </row>
     <row r="72" spans="12:12">
-      <c r="L72" s="67"/>
+      <c r="L72" s="66"/>
     </row>
     <row r="73" spans="12:12">
-      <c r="L73" s="67"/>
+      <c r="L73" s="66"/>
     </row>
     <row r="74" spans="12:12">
-      <c r="L74" s="67"/>
+      <c r="L74" s="66"/>
     </row>
     <row r="75" spans="12:12">
-      <c r="L75" s="67"/>
+      <c r="L75" s="66"/>
     </row>
     <row r="76" spans="12:12">
-      <c r="L76" s="67"/>
+      <c r="L76" s="66"/>
     </row>
     <row r="77" spans="12:12">
-      <c r="L77" s="67"/>
+      <c r="L77" s="66"/>
     </row>
     <row r="78" spans="12:12">
-      <c r="L78" s="67"/>
+      <c r="L78" s="66"/>
     </row>
     <row r="79" spans="12:12">
-      <c r="L79" s="67"/>
+      <c r="L79" s="66"/>
     </row>
     <row r="80" spans="12:12">
-      <c r="L80" s="67"/>
+      <c r="L80" s="66"/>
     </row>
     <row r="81" spans="1:14">
-      <c r="L81" s="67"/>
+      <c r="L81" s="66"/>
     </row>
     <row r="82" spans="1:14">
-      <c r="L82" s="67"/>
+      <c r="L82" s="66"/>
     </row>
     <row r="83" spans="1:14">
-      <c r="L83" s="67"/>
+      <c r="L83" s="66"/>
     </row>
     <row r="84" spans="1:14">
-      <c r="A84" s="67" t="s">
+      <c r="A84" s="66" t="s">
         <v>123</v>
       </c>
-      <c r="C84" s="67" t="s">
+      <c r="C84" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="F84" s="67" t="s">
+      <c r="F84" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="K84" s="73" t="s">
+      <c r="K84" s="72" t="s">
         <v>126</v>
       </c>
-      <c r="L84" s="67"/>
-      <c r="N84" s="67" t="s">
+      <c r="L84" s="66"/>
+      <c r="N84" s="66" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="85" spans="1:14">
-      <c r="L85" s="67"/>
+      <c r="L85" s="66"/>
     </row>
     <row r="86" spans="1:14">
-      <c r="A86" s="67" t="s">
+      <c r="A86" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="L86" s="67"/>
+      <c r="L86" s="66"/>
     </row>
     <row r="87" spans="1:14">
-      <c r="A87" s="67" t="s">
+      <c r="A87" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="L87" s="67"/>
+      <c r="L87" s="66"/>
     </row>
     <row r="88" spans="1:14">
-      <c r="A88" s="67" t="s">
+      <c r="A88" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="L88" s="67"/>
+      <c r="L88" s="66"/>
     </row>
     <row r="89" spans="1:14">
-      <c r="A89" s="67" t="s">
+      <c r="A89" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="L89" s="67"/>
+      <c r="L89" s="66"/>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="67" t="s">
+      <c r="A90" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="L90" s="67"/>
+      <c r="L90" s="66"/>
     </row>
     <row r="91" spans="1:14">
-      <c r="A91" s="67" t="s">
+      <c r="A91" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="L91" s="67"/>
+      <c r="L91" s="66"/>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92" s="67" t="s">
+      <c r="A92" s="66" t="s">
         <v>138</v>
       </c>
-      <c r="L92" s="67"/>
+      <c r="L92" s="66"/>
     </row>
     <row r="93" spans="1:14">
-      <c r="A93" s="67" t="s">
+      <c r="A93" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="L93" s="67"/>
+      <c r="L93" s="66"/>
     </row>
     <row r="94" spans="1:14">
-      <c r="A94" s="67" t="s">
+      <c r="A94" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="L94" s="67"/>
+      <c r="L94" s="66"/>
     </row>
     <row r="95" spans="1:14">
-      <c r="A95" s="67" t="s">
+      <c r="A95" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="L95" s="67"/>
+      <c r="L95" s="66"/>
     </row>
     <row r="96" spans="1:14">
-      <c r="A96" s="67" t="s">
+      <c r="A96" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="L96" s="67"/>
+      <c r="L96" s="66"/>
     </row>
     <row r="97" spans="1:12">
-      <c r="A97" s="67" t="s">
+      <c r="A97" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="L97" s="67"/>
+      <c r="L97" s="66"/>
     </row>
     <row r="98" spans="1:12">
-      <c r="A98" s="67" t="s">
+      <c r="A98" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="L98" s="67"/>
+      <c r="L98" s="66"/>
     </row>
     <row r="99" spans="1:12">
-      <c r="A99" s="67" t="s">
+      <c r="A99" s="66" t="s">
         <v>144</v>
       </c>
-      <c r="L99" s="67"/>
+      <c r="L99" s="66"/>
     </row>
     <row r="100" spans="1:12">
-      <c r="A100" s="67" t="s">
+      <c r="A100" s="66" t="s">
         <v>145</v>
       </c>
-      <c r="L100" s="67"/>
+      <c r="L100" s="66"/>
     </row>
     <row r="101" spans="1:12">
-      <c r="A101" s="67" t="s">
+      <c r="A101" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="L101" s="67"/>
+      <c r="L101" s="66"/>
     </row>
     <row r="102" spans="1:12">
-      <c r="A102" s="67" t="s">
+      <c r="A102" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="L102" s="67"/>
+      <c r="L102" s="66"/>
     </row>
     <row r="103" spans="1:12">
-      <c r="A103" s="67" t="s">
+      <c r="A103" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="L103" s="67"/>
+      <c r="L103" s="66"/>
     </row>
     <row r="104" spans="1:12">
-      <c r="A104" s="67" t="s">
+      <c r="A104" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="L104" s="67"/>
+      <c r="L104" s="66"/>
     </row>
     <row r="105" spans="1:12">
-      <c r="A105" s="67" t="s">
+      <c r="A105" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="L105" s="67"/>
+      <c r="L105" s="66"/>
     </row>
     <row r="106" spans="1:12">
-      <c r="A106" s="67" t="s">
+      <c r="A106" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="L106" s="67"/>
+      <c r="L106" s="66"/>
     </row>
     <row r="107" spans="1:12">
-      <c r="A107" s="67" t="s">
+      <c r="A107" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="L107" s="67"/>
+      <c r="L107" s="66"/>
     </row>
     <row r="108" spans="1:12">
-      <c r="A108" s="67" t="s">
+      <c r="A108" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="L108" s="67"/>
+      <c r="L108" s="66"/>
     </row>
     <row r="109" spans="1:12">
-      <c r="A109" s="67" t="s">
+      <c r="A109" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="L109" s="67"/>
+      <c r="L109" s="66"/>
     </row>
     <row r="110" spans="1:12">
-      <c r="A110" s="67" t="s">
+      <c r="A110" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="L110" s="67"/>
+      <c r="L110" s="66"/>
     </row>
     <row r="111" spans="1:12">
-      <c r="A111" s="67" t="s">
+      <c r="A111" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="L111" s="67"/>
+      <c r="L111" s="66"/>
     </row>
     <row r="112" spans="1:12">
-      <c r="A112" s="67" t="s">
+      <c r="A112" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="L112" s="67"/>
+      <c r="L112" s="66"/>
     </row>
     <row r="113" spans="1:12">
-      <c r="A113" s="67" t="s">
+      <c r="A113" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="L113" s="67"/>
+      <c r="L113" s="66"/>
     </row>
     <row r="114" spans="1:12">
-      <c r="A114" s="67" t="s">
+      <c r="A114" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="L114" s="67"/>
+      <c r="L114" s="66"/>
     </row>
     <row r="115" spans="1:12">
-      <c r="A115" s="67" t="s">
+      <c r="A115" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="L115" s="67"/>
+      <c r="L115" s="66"/>
     </row>
     <row r="116" spans="1:12">
-      <c r="A116" s="67" t="s">
+      <c r="A116" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="L116" s="67"/>
+      <c r="L116" s="66"/>
     </row>
     <row r="117" spans="1:12">
-      <c r="A117" s="67" t="s">
+      <c r="A117" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="L117" s="67"/>
+      <c r="L117" s="66"/>
     </row>
     <row r="118" spans="1:12">
-      <c r="A118" s="67" t="s">
+      <c r="A118" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="L118" s="67"/>
+      <c r="L118" s="66"/>
     </row>
     <row r="119" spans="1:12">
-      <c r="A119" s="67" t="s">
+      <c r="A119" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="L119" s="67"/>
+      <c r="L119" s="66"/>
     </row>
     <row r="120" spans="1:12">
-      <c r="A120" s="67" t="s">
+      <c r="A120" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="L120" s="67"/>
+      <c r="L120" s="66"/>
     </row>
     <row r="121" spans="1:12">
-      <c r="A121" s="67" t="s">
+      <c r="A121" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="L121" s="67"/>
+      <c r="L121" s="66"/>
     </row>
     <row r="122" spans="1:12">
-      <c r="A122" s="67" t="s">
+      <c r="A122" s="66" t="s">
         <v>147</v>
       </c>
-      <c r="L122" s="67"/>
+      <c r="L122" s="66"/>
     </row>
     <row r="123" spans="1:12">
-      <c r="A123" s="67" t="s">
+      <c r="A123" s="66" t="s">
         <v>148</v>
       </c>
-      <c r="L123" s="67"/>
+      <c r="L123" s="66"/>
     </row>
     <row r="124" spans="1:12">
-      <c r="A124" s="67" t="s">
+      <c r="A124" s="66" t="s">
         <v>149</v>
       </c>
-      <c r="L124" s="67"/>
+      <c r="L124" s="66"/>
     </row>
     <row r="125" spans="1:12">
-      <c r="A125" s="67" t="s">
+      <c r="A125" s="66" t="s">
         <v>150</v>
       </c>
-      <c r="L125" s="67"/>
+      <c r="L125" s="66"/>
     </row>
     <row r="126" spans="1:12">
-      <c r="A126" s="67" t="s">
+      <c r="A126" s="66" t="s">
         <v>151</v>
       </c>
-      <c r="L126" s="67"/>
+      <c r="L126" s="66"/>
     </row>
     <row r="127" spans="1:12">
-      <c r="A127" s="67" t="s">
+      <c r="A127" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="L127" s="67"/>
+      <c r="L127" s="66"/>
     </row>
     <row r="128" spans="1:12">
-      <c r="A128" s="67" t="s">
+      <c r="A128" s="66" t="s">
         <v>153</v>
       </c>
-      <c r="L128" s="67"/>
+      <c r="L128" s="66"/>
     </row>
     <row r="129" spans="1:12">
-      <c r="A129" s="67" t="s">
+      <c r="A129" s="66" t="s">
         <v>154</v>
       </c>
-      <c r="L129" s="67"/>
+      <c r="L129" s="66"/>
     </row>
     <row r="130" spans="1:12">
-      <c r="A130" s="67" t="s">
+      <c r="A130" s="66" t="s">
         <v>155</v>
       </c>
-      <c r="L130" s="67"/>
+      <c r="L130" s="66"/>
     </row>
     <row r="131" spans="1:12">
-      <c r="A131" s="67" t="s">
+      <c r="A131" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="L131" s="67"/>
+      <c r="L131" s="66"/>
     </row>
     <row r="132" spans="1:12">
-      <c r="A132" s="67" t="s">
+      <c r="A132" s="66" t="s">
         <v>157</v>
       </c>
-      <c r="L132" s="67"/>
+      <c r="L132" s="66"/>
     </row>
     <row r="133" spans="1:12">
-      <c r="A133" s="67" t="s">
+      <c r="A133" s="66" t="s">
         <v>158</v>
       </c>
-      <c r="L133" s="67"/>
+      <c r="L133" s="66"/>
     </row>
     <row r="134" spans="1:12">
-      <c r="A134" s="67" t="s">
+      <c r="A134" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="L134" s="67"/>
+      <c r="L134" s="66"/>
     </row>
     <row r="135" spans="1:12">
-      <c r="A135" s="67" t="s">
+      <c r="A135" s="66" t="s">
         <v>160</v>
       </c>
-      <c r="L135" s="67"/>
+      <c r="L135" s="66"/>
     </row>
     <row r="136" spans="1:12">
-      <c r="A136" s="67" t="s">
+      <c r="A136" s="66" t="s">
         <v>161</v>
       </c>
-      <c r="L136" s="67"/>
+      <c r="L136" s="66"/>
     </row>
     <row r="137" spans="1:12">
-      <c r="A137" s="67" t="s">
+      <c r="A137" s="66" t="s">
         <v>162</v>
       </c>
-      <c r="L137" s="67"/>
+      <c r="L137" s="66"/>
     </row>
     <row r="138" spans="1:12">
-      <c r="A138" s="67" t="s">
+      <c r="A138" s="66" t="s">
         <v>163</v>
       </c>
-      <c r="L138" s="67"/>
+      <c r="L138" s="66"/>
     </row>
     <row r="139" spans="1:12">
-      <c r="A139" s="67" t="s">
+      <c r="A139" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="L139" s="67"/>
+      <c r="L139" s="66"/>
     </row>
     <row r="140" spans="1:12">
-      <c r="A140" s="67" t="s">
+      <c r="A140" s="66" t="s">
         <v>165</v>
       </c>
-      <c r="L140" s="67"/>
+      <c r="L140" s="66"/>
     </row>
     <row r="141" spans="1:12">
-      <c r="A141" s="67" t="s">
+      <c r="A141" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="L141" s="67"/>
+      <c r="L141" s="66"/>
     </row>
     <row r="142" spans="1:12">
-      <c r="A142" s="67" t="s">
+      <c r="A142" s="66" t="s">
         <v>167</v>
       </c>
-      <c r="L142" s="67"/>
+      <c r="L142" s="66"/>
     </row>
     <row r="143" spans="1:12">
-      <c r="A143" s="67" t="s">
+      <c r="A143" s="66" t="s">
         <v>168</v>
       </c>
-      <c r="L143" s="67"/>
+      <c r="L143" s="66"/>
     </row>
     <row r="144" spans="1:12">
-      <c r="A144" s="67" t="s">
+      <c r="A144" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="L144" s="67"/>
+      <c r="L144" s="66"/>
     </row>
     <row r="145" spans="1:12">
-      <c r="A145" s="67" t="s">
+      <c r="A145" s="66" t="s">
         <v>170</v>
       </c>
-      <c r="L145" s="67"/>
+      <c r="L145" s="66"/>
     </row>
     <row r="146" spans="1:12">
-      <c r="A146" s="67" t="s">
+      <c r="A146" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="L146" s="67"/>
+      <c r="L146" s="66"/>
     </row>
     <row r="147" spans="1:12">
-      <c r="A147" s="67" t="s">
+      <c r="A147" s="66" t="s">
         <v>172</v>
       </c>
-      <c r="L147" s="67"/>
+      <c r="L147" s="66"/>
     </row>
     <row r="148" spans="1:12">
-      <c r="A148" s="67" t="s">
+      <c r="A148" s="66" t="s">
         <v>173</v>
       </c>
-      <c r="L148" s="67"/>
+      <c r="L148" s="66"/>
     </row>
     <row r="149" spans="1:12">
-      <c r="A149" s="67" t="s">
+      <c r="A149" s="66" t="s">
         <v>174</v>
       </c>
-      <c r="L149" s="67"/>
+      <c r="L149" s="66"/>
     </row>
     <row r="150" spans="1:12">
-      <c r="A150" s="67" t="s">
+      <c r="A150" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="L150" s="67"/>
+      <c r="L150" s="66"/>
     </row>
     <row r="151" spans="1:12">
-      <c r="A151" s="67" t="s">
+      <c r="A151" s="66" t="s">
         <v>176</v>
       </c>
-      <c r="L151" s="67"/>
+      <c r="L151" s="66"/>
     </row>
     <row r="152" spans="1:12">
-      <c r="A152" s="67" t="s">
+      <c r="A152" s="66" t="s">
         <v>177</v>
       </c>
-      <c r="L152" s="67"/>
+      <c r="L152" s="66"/>
     </row>
     <row r="153" spans="1:12">
-      <c r="A153" s="67" t="s">
+      <c r="A153" s="66" t="s">
         <v>178</v>
       </c>
-      <c r="L153" s="67"/>
+      <c r="L153" s="66"/>
     </row>
     <row r="154" spans="1:12">
-      <c r="A154" s="67" t="s">
+      <c r="A154" s="66" t="s">
         <v>179</v>
       </c>
-      <c r="L154" s="67"/>
+      <c r="L154" s="66"/>
     </row>
     <row r="155" spans="1:12">
-      <c r="A155" s="67" t="s">
+      <c r="A155" s="66" t="s">
         <v>180</v>
       </c>
-      <c r="L155" s="67"/>
+      <c r="L155" s="66"/>
     </row>
     <row r="156" spans="1:12">
-      <c r="A156" s="67" t="s">
+      <c r="A156" s="66" t="s">
         <v>181</v>
       </c>
-      <c r="L156" s="67"/>
+      <c r="L156" s="66"/>
     </row>
     <row r="157" spans="1:12">
-      <c r="A157" s="67" t="s">
+      <c r="A157" s="66" t="s">
         <v>182</v>
       </c>
-      <c r="L157" s="67"/>
+      <c r="L157" s="66"/>
     </row>
     <row r="158" spans="1:12">
-      <c r="A158" s="67" t="s">
+      <c r="A158" s="66" t="s">
         <v>183</v>
       </c>
-      <c r="L158" s="67"/>
+      <c r="L158" s="66"/>
     </row>
     <row r="159" spans="1:12">
-      <c r="A159" s="67" t="s">
+      <c r="A159" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="L159" s="67"/>
+      <c r="L159" s="66"/>
     </row>
     <row r="160" spans="1:12">
-      <c r="A160" s="67" t="s">
+      <c r="A160" s="66" t="s">
         <v>185</v>
       </c>
-      <c r="L160" s="67"/>
+      <c r="L160" s="66"/>
     </row>
     <row r="161" spans="1:12">
-      <c r="A161" s="67" t="s">
+      <c r="A161" s="66" t="s">
         <v>186</v>
       </c>
-      <c r="L161" s="67"/>
+      <c r="L161" s="66"/>
     </row>
     <row r="162" spans="1:12">
-      <c r="A162" s="67" t="s">
+      <c r="A162" s="66" t="s">
         <v>187</v>
       </c>
-      <c r="L162" s="67"/>
+      <c r="L162" s="66"/>
     </row>
     <row r="163" spans="1:12">
-      <c r="A163" s="67" t="s">
+      <c r="A163" s="66" t="s">
         <v>188</v>
       </c>
-      <c r="L163" s="67"/>
+      <c r="L163" s="66"/>
     </row>
     <row r="164" spans="1:12">
-      <c r="A164" s="67" t="s">
+      <c r="A164" s="66" t="s">
         <v>189</v>
       </c>
-      <c r="L164" s="67"/>
+      <c r="L164" s="66"/>
     </row>
     <row r="165" spans="1:12">
-      <c r="A165" s="67" t="s">
+      <c r="A165" s="66" t="s">
         <v>190</v>
       </c>
-      <c r="L165" s="67"/>
+      <c r="L165" s="66"/>
     </row>
     <row r="166" spans="1:12">
-      <c r="A166" s="67" t="s">
+      <c r="A166" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="L166" s="67"/>
+      <c r="L166" s="66"/>
     </row>
     <row r="167" spans="1:12">
-      <c r="A167" s="67" t="s">
+      <c r="A167" s="66" t="s">
         <v>192</v>
       </c>
-      <c r="L167" s="67"/>
+      <c r="L167" s="66"/>
     </row>
     <row r="168" spans="1:12">
-      <c r="A168" s="67" t="s">
+      <c r="A168" s="66" t="s">
         <v>193</v>
       </c>
-      <c r="L168" s="67"/>
+      <c r="L168" s="66"/>
     </row>
     <row r="169" spans="1:12">
-      <c r="A169" s="67" t="s">
+      <c r="A169" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="L169" s="67"/>
+      <c r="L169" s="66"/>
     </row>
     <row r="170" spans="1:12">
-      <c r="A170" s="67" t="s">
+      <c r="A170" s="66" t="s">
         <v>195</v>
       </c>
-      <c r="L170" s="67"/>
+      <c r="L170" s="66"/>
     </row>
     <row r="171" spans="1:12">
-      <c r="A171" s="67" t="s">
+      <c r="A171" s="66" t="s">
         <v>196</v>
       </c>
-      <c r="L171" s="67"/>
+      <c r="L171" s="66"/>
     </row>
     <row r="172" spans="1:12">
-      <c r="A172" s="67" t="s">
+      <c r="A172" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="L172" s="67"/>
+      <c r="L172" s="66"/>
     </row>
     <row r="173" spans="1:12">
-      <c r="A173" s="67" t="s">
+      <c r="A173" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="L173" s="67"/>
+      <c r="L173" s="66"/>
     </row>
     <row r="174" spans="1:12">
-      <c r="A174" s="67" t="s">
+      <c r="A174" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="L174" s="67"/>
+      <c r="L174" s="66"/>
     </row>
     <row r="175" spans="1:12">
-      <c r="A175" s="67" t="s">
+      <c r="A175" s="66" t="s">
         <v>200</v>
       </c>
-      <c r="L175" s="67"/>
+      <c r="L175" s="66"/>
     </row>
     <row r="176" spans="1:12">
-      <c r="L176" s="67"/>
+      <c r="L176" s="66"/>
     </row>
     <row r="177" spans="12:12">
-      <c r="L177" s="67"/>
+      <c r="L177" s="66"/>
     </row>
     <row r="178" spans="12:12">
-      <c r="L178" s="67"/>
+      <c r="L178" s="66"/>
     </row>
     <row r="179" spans="12:12">
-      <c r="L179" s="67"/>
+      <c r="L179" s="66"/>
     </row>
     <row r="180" spans="12:12">
-      <c r="L180" s="67"/>
+      <c r="L180" s="66"/>
     </row>
     <row r="181" spans="12:12">
-      <c r="L181" s="67"/>
+      <c r="L181" s="66"/>
     </row>
     <row r="182" spans="12:12">
-      <c r="L182" s="67"/>
+      <c r="L182" s="66"/>
     </row>
     <row r="183" spans="12:12">
-      <c r="L183" s="67"/>
+      <c r="L183" s="66"/>
     </row>
     <row r="184" spans="12:12">
-      <c r="L184" s="67"/>
+      <c r="L184" s="66"/>
     </row>
     <row r="185" spans="12:12">
-      <c r="L185" s="67"/>
+      <c r="L185" s="66"/>
     </row>
     <row r="186" spans="12:12">
-      <c r="L186" s="67"/>
+      <c r="L186" s="66"/>
     </row>
     <row r="187" spans="12:12">
-      <c r="L187" s="67"/>
+      <c r="L187" s="66"/>
     </row>
     <row r="188" spans="12:12">
-      <c r="L188" s="67"/>
+      <c r="L188" s="66"/>
     </row>
     <row r="189" spans="12:12">
-      <c r="L189" s="67"/>
+      <c r="L189" s="66"/>
     </row>
     <row r="190" spans="12:12">
-      <c r="L190" s="67"/>
+      <c r="L190" s="66"/>
     </row>
     <row r="191" spans="12:12">
-      <c r="L191" s="67"/>
+      <c r="L191" s="66"/>
     </row>
     <row r="192" spans="12:12">
-      <c r="L192" s="67"/>
+      <c r="L192" s="66"/>
     </row>
     <row r="193" spans="12:12">
-      <c r="L193" s="67"/>
+      <c r="L193" s="66"/>
     </row>
     <row r="194" spans="12:12">
-      <c r="L194" s="67"/>
+      <c r="L194" s="66"/>
     </row>
     <row r="195" spans="12:12">
-      <c r="L195" s="67"/>
+      <c r="L195" s="66"/>
     </row>
     <row r="196" spans="12:12">
-      <c r="L196" s="67"/>
+      <c r="L196" s="66"/>
     </row>
     <row r="197" spans="12:12">
-      <c r="L197" s="67"/>
+      <c r="L197" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -9494,13 +9789,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M43">
@@ -9523,6 +9811,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>